<commit_message>
Fix import in analyser + zfillÃ
</commit_message>
<xml_diff>
--- a/excel/run.xlsx
+++ b/excel/run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Loup\Python\Projet\LiveSplit_Sync\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE39D0B1-8D02-4553-9DD0-1DEEAF7DB0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00936CC-CF9D-464A-A148-4299624DEDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aaaaaa" sheetId="3" r:id="rId1"/>
@@ -136,12 +136,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,15 +503,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6AF669-E037-4A4F-8A10-1CA0D4F248E8}">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="17.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" style="5"/>
     <col min="9" max="9" width="11.453125" style="1"/>
   </cols>
   <sheetData>
@@ -519,7 +526,7 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
@@ -547,15 +554,8 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="3"/>
-    </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -563,89 +563,106 @@
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="J14" s="4"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="3"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="3"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="3"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B24" s="3"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -654,7 +671,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -663,7 +680,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -672,7 +689,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -681,23 +698,31 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
-      <c r="D32" s="4"/>
+      <c r="D32" s="6"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="2"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
@@ -707,74 +732,67 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
-      <c r="D37" s="4"/>
+      <c r="D37" s="6"/>
       <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
-      <c r="D38" s="4"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B39" s="3"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B40" s="3"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="J38" s="4"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="6"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="J41" s="4"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
-      <c r="D42" s="4"/>
+      <c r="D42" s="6"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="J42" s="4"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+      <c r="D43" s="6"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
+      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
-      <c r="D45" s="4"/>
+      <c r="D45" s="6"/>
       <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B46" s="3"/>
-      <c r="D46" s="4"/>
+      <c r="D46" s="6"/>
       <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
-      <c r="D47" s="4"/>
+      <c r="D47" s="6"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -783,164 +801,163 @@
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48" s="3"/>
-      <c r="D48" s="4"/>
+      <c r="D48" s="6"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B51" s="3"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B52" s="3"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B49" s="3"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B50" s="3"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B53" s="3"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B54" s="3"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" s="3"/>
-      <c r="D55" s="4"/>
+      <c r="D55" s="6"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-      <c r="J55" s="4"/>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" s="3"/>
-      <c r="D56" s="4"/>
+      <c r="D56" s="6"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" s="3"/>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" s="3"/>
-      <c r="D58" s="4"/>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B59" s="3"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B60" s="3"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="3"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="J61" s="4"/>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="3"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="J62" s="4"/>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="3"/>
-      <c r="D63" s="4"/>
+      <c r="D63" s="6"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="J63" s="4"/>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B64" s="3"/>
-      <c r="D64" s="4"/>
+      <c r="D64" s="6"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="J64" s="4"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D65" s="4"/>
+      <c r="B65" s="3"/>
+      <c r="D65" s="6"/>
       <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="J65" s="4"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="J66" s="4"/>
+      <c r="B66" s="3"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="4"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B67" s="3"/>
-      <c r="D67" s="4"/>
+      <c r="D67" s="6"/>
       <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="2"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B68" s="3"/>
-      <c r="D68" s="4"/>
+      <c r="D68" s="6"/>
       <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="2"/>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B69" s="3"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B70" s="3"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B71" s="3"/>
-      <c r="D71" s="4"/>
+      <c r="D71" s="6"/>
       <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="2"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B72" s="3"/>
-      <c r="D72" s="4"/>
+      <c r="D72" s="6"/>
       <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="2"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B73" s="3"/>
-      <c r="D73" s="4"/>
+      <c r="D73" s="6"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="2"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B74" s="3"/>
-      <c r="D74" s="4"/>
+      <c r="D74" s="6"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="2"/>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B75" s="3"/>
-      <c r="D75" s="4"/>
+      <c r="D75" s="6"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -949,173 +966,339 @@
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B76" s="3"/>
-      <c r="D76" s="4"/>
+      <c r="D76" s="6"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B77" s="3"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="J77" s="4"/>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B78" s="3"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="J78" s="4"/>
-    </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B79" s="3"/>
-      <c r="D79" s="4"/>
+      <c r="D79" s="6"/>
       <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="2"/>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B80" s="3"/>
-      <c r="D80" s="4"/>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B81" s="3"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="4"/>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B82" s="3"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="2"/>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D80" s="6"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="2"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B83" s="3"/>
-      <c r="D83" s="4"/>
+      <c r="D83" s="6"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
-      <c r="I83" s="2"/>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J83" s="4"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B84" s="3"/>
-      <c r="D84" s="4"/>
+      <c r="D84" s="6"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
       <c r="I84" s="2"/>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B85" s="3"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="J85" s="4"/>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D85" s="6"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B86" s="3"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="2"/>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B87" s="3"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="2"/>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B88" s="3"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="2"/>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D86" s="6"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B89" s="3"/>
-      <c r="D89" s="4"/>
+      <c r="D89" s="6"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
-      <c r="I89" s="2"/>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J89" s="4"/>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B90" s="3"/>
-      <c r="D90" s="4"/>
+      <c r="D90" s="6"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
-      <c r="I90" s="2"/>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J90" s="4"/>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B91" s="3"/>
-      <c r="D91" s="4"/>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D91" s="6"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="J91" s="4"/>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B92" s="3"/>
-      <c r="C92" s="4"/>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D93" s="4"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="J92" s="4"/>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D93" s="6"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="J93" s="4"/>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B94" s="3"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
-      <c r="I94" s="2"/>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="J94" s="4"/>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B95" s="3"/>
-      <c r="D95" s="4"/>
+      <c r="D95" s="6"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B96" s="3"/>
-      <c r="D96" s="4"/>
+      <c r="D96" s="6"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
-    </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.35">
-      <c r="I105" s="2"/>
+      <c r="I96" s="2"/>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B99" s="3"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="2"/>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B100" s="3"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="2"/>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B101" s="3"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="2"/>
+    </row>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B102" s="3"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="2"/>
+    </row>
+    <row r="103" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B103" s="3"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="J103" s="4"/>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B104" s="3"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="J104" s="4"/>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B105" s="3"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="J105" s="4"/>
+    </row>
+    <row r="106" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B106" s="3"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="J106" s="4"/>
+    </row>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B107" s="3"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="4"/>
+    </row>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B108" s="3"/>
+      <c r="D108" s="6"/>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B109" s="3"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="4"/>
+    </row>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B110" s="3"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="2"/>
+    </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B111" s="3"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="2"/>
+    </row>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B112" s="3"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="I112" s="2"/>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B113" s="3"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="J113" s="4"/>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B114" s="3"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="2"/>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B115" s="3"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="2"/>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B116" s="3"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="2"/>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B117" s="3"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="2"/>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B118" s="3"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="2"/>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B119" s="3"/>
+      <c r="D119" s="6"/>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B120" s="3"/>
+      <c r="C120" s="4"/>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D121" s="6"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="J121" s="4"/>
+    </row>
+    <row r="122" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B122" s="3"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="2"/>
+    </row>
+    <row r="123" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B123" s="3"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="2"/>
+    </row>
+    <row r="124" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B124" s="3"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
+    </row>
+    <row r="133" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I133" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>